<commit_message>
fix scaling of 2024 logs
</commit_message>
<xml_diff>
--- a/logs/2024/All Quiet on the Western Front - Erich Maria Remarque.xlsx
+++ b/logs/2024/All Quiet on the Western Front - Erich Maria Remarque.xlsx
@@ -430,7 +430,7 @@
         <v>45439</v>
       </c>
       <c r="B1" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
@@ -438,7 +438,7 @@
         <v>45441</v>
       </c>
       <c r="B2" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
@@ -446,7 +446,7 @@
         <v>45443</v>
       </c>
       <c r="B3" t="n">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4">
@@ -454,7 +454,7 @@
         <v>45444</v>
       </c>
       <c r="B4" t="n">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>